<commit_message>
Streamlit App Work: Mainly worked on the Classification Page * Updated models to scikit-learn:1.0.2 so i had to update the model files and their metrics in data/ * Minor details added to Reference and Dataset pages * Added the ability to make predictions using the models in the Classification page. Just with the chemical descriptors currently
</commit_message>
<xml_diff>
--- a/Streamlit_App/data/Metrics/Classification_Models_CD_SE_I_Testing_Metrics.xlsx
+++ b/Streamlit_App/data/Metrics/Classification_Models_CD_SE_I_Testing_Metrics.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jogeo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jogeo\Desktop\Project\Blood-Brain-Barrier-Drug-Prediction\Streamlit_App\data\Metrics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CF021E7-044B-4D69-A1D4-B2A233530C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{923A1E8B-E8AC-409C-88E6-20DFCD295DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0CD68A16-22DD-4DC5-9249-015F8712004B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>Classification Models – Chemical Descriptors, Side Effects and Indications With Feature Selection</t>
   </si>
@@ -89,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0000000000"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -115,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -188,36 +188,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -227,21 +210,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -560,50 +530,50 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" ht="54" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="7">
@@ -622,9 +592,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="4" t="s">
+    <row r="4" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="7">
@@ -643,9 +615,11 @@
         <v>0.41910986930593003</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="7">
@@ -664,9 +638,11 @@
         <v>0.52952809732294404</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="7">
@@ -685,9 +661,11 @@
         <v>0.64310344827586197</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="7">
@@ -706,9 +684,11 @@
         <v>0.67158620053623097</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="7">
@@ -727,9 +707,11 @@
         <v>0.47788747292810302</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="7">
@@ -749,9 +731,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>